<commit_message>
alles fertig außer brille
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/gtsrb_notebooks/experiments_gtsrb.xlsx
+++ b/examples/masterarbeit/gtsrb_notebooks/experiments_gtsrb.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\gtsrb_notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E627E8-2A17-4035-8C7D-D01AC679E937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB448FFC-E5DD-429F-98A3-BDDC062C5588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="103">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -129,12 +130,6 @@
     <t>unnötig</t>
   </si>
   <si>
-    <t>exp_gtsrb_20200227-092839</t>
-  </si>
-  <si>
-    <t>exp_gtsrb_20200226-181550</t>
-  </si>
-  <si>
     <t>exp_gtsrb_20200227-145350</t>
   </si>
   <si>
@@ -316,13 +311,43 @@
   </si>
   <si>
     <t>die da kennen nur die non-iid klassen</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200318-203814</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200318-203612</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200319-161053</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200319-173620</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200320-003449</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200320-085236</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200320-090424</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200320-225526</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200321-011532</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +412,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +435,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -445,13 +482,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,11 +498,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Ausgabe" xfId="3" builtinId="21"/>
     <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -777,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -982,10 +1022,10 @@
         <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
@@ -1010,16 +1050,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1033,16 +1073,16 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1056,19 +1096,19 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
@@ -1083,16 +1123,16 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1106,16 +1146,16 @@
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1129,19 +1169,19 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
@@ -1156,16 +1196,16 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1179,16 +1219,16 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
@@ -1206,16 +1246,16 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1229,16 +1269,16 @@
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1252,16 +1292,16 @@
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1275,13 +1315,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
@@ -1315,7 +1355,7 @@
         <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
@@ -1343,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -1371,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I31"/>
       <c r="J31"/>
@@ -1491,7 +1531,7 @@
         <v>30</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1520,7 +1560,7 @@
         <v>30</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1549,7 +1589,7 @@
         <v>30</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1578,90 +1618,55 @@
         <v>30</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="7">
-        <v>4</v>
-      </c>
-      <c r="C41" s="7">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="7">
-        <v>25</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="7">
-        <v>4</v>
-      </c>
-      <c r="C42" s="7">
-        <v>1</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="7">
-        <v>50</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="7">
-        <v>4</v>
-      </c>
-      <c r="C43" s="7">
-        <v>1</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="7">
-        <v>75</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>31</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42"/>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="1">
+        <v>100</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1">
         <v>4</v>
@@ -1679,18 +1684,18 @@
         <v>10</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" s="1">
         <v>4</v>
@@ -1708,32 +1713,82 @@
         <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I46"/>
-      <c r="J46"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>20</v>
-      </c>
-      <c r="I47"/>
-      <c r="J47"/>
+        <v>37</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1">
+        <v>100</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1">
+        <v>100</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -1748,16 +1803,13 @@
         <v>10</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1765,7 +1817,7 @@
         <v>7</v>
       </c>
       <c r="B49" s="1">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -1786,7 +1838,7 @@
         <v>30</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1794,7 +1846,7 @@
         <v>7</v>
       </c>
       <c r="B50" s="1">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
@@ -1812,436 +1864,402 @@
         <v>12</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="1">
-        <v>4</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="1">
-        <v>100</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="B53" s="7">
+        <v>4</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="7">
+        <v>100</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="54" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="7">
+        <v>100</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="1">
-        <v>9</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="1">
-        <v>100</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="1">
-        <v>9</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1">
-        <v>100</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="1" t="s">
+      <c r="B55" s="7">
+        <v>9</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="7">
+        <v>100</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" s="1">
-        <v>19</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1">
-        <v>100</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="1">
-        <v>19</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1">
-        <v>100</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I56"/>
-      <c r="J56"/>
+    </row>
+    <row r="56" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="7">
+        <v>9</v>
+      </c>
+      <c r="C56" s="7">
+        <v>1</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="7">
+        <v>100</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I58"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="1">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="1">
+        <v>25</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="1">
+        <v>4</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="1">
+        <v>50</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="1">
+        <v>75</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="1">
+        <v>4</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="1">
+        <v>100</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="1">
+        <v>9</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="1">
+        <v>100</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="8">
+        <v>8</v>
+      </c>
+      <c r="C65" s="8">
+        <v>2</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="8">
+        <v>100</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="8">
         <v>7</v>
       </c>
-      <c r="B58" s="7">
-        <v>4</v>
-      </c>
-      <c r="C58" s="7">
-        <v>1</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="7">
-        <v>100</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" s="7">
-        <v>4</v>
-      </c>
-      <c r="C59" s="7">
-        <v>1</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="7">
-        <v>100</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" s="7">
-        <v>9</v>
-      </c>
-      <c r="C60" s="7">
-        <v>1</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="7">
-        <v>100</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="7">
-        <v>9</v>
-      </c>
-      <c r="C61" s="7">
-        <v>1</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="7">
-        <v>100</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I62"/>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="I63"/>
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>18</v>
-      </c>
-      <c r="I64"/>
-      <c r="J64"/>
-    </row>
-    <row r="65" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="1">
-        <v>4</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="1">
-        <v>25</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="1">
-        <v>4</v>
-      </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="1">
-        <v>50</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" s="1">
-        <v>4</v>
-      </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="1">
-        <v>75</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B68" s="1">
-        <v>4</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="1">
-        <v>100</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="I69"/>
-      <c r="J69"/>
-    </row>
-    <row r="70" spans="1:10" s="1" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" s="1">
-        <v>4</v>
-      </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="1">
-        <v>12.5</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C66" s="8">
+        <v>3</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="8">
+        <v>100</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="8">
+        <v>3</v>
+      </c>
+      <c r="C67" s="8">
+        <v>2</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="8">
+        <v>100</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="8">
+        <v>2</v>
+      </c>
+      <c r="C68" s="8">
+        <v>3</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="8">
+        <v>100</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="I70"/>
+      <c r="J70"/>
     </row>
     <row r="71" spans="1:10" s="1" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
@@ -2266,16 +2284,16 @@
         <v>13</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="1" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>9</v>
       </c>
       <c r="E72" s="1">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>22</v>
@@ -2298,13 +2316,13 @@
         <v>13</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2330,10 +2348,13 @@
         <v>13</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2350,7 +2371,7 @@
         <v>9</v>
       </c>
       <c r="E74" s="1">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>22</v>
@@ -2359,10 +2380,10 @@
         <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2388,10 +2409,10 @@
         <v>13</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2408,7 +2429,7 @@
         <v>9</v>
       </c>
       <c r="E76" s="1">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>22</v>
@@ -2417,10 +2438,10 @@
         <v>13</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2446,13 +2467,10 @@
         <v>13</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2469,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="E78" s="1">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>22</v>
@@ -2478,10 +2496,13 @@
         <v>13</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2507,13 +2528,10 @@
         <v>13</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2530,7 +2548,7 @@
         <v>9</v>
       </c>
       <c r="E80" s="1">
-        <v>12.5</v>
+        <v>100</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>22</v>
@@ -2539,10 +2557,13 @@
         <v>13</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2559,7 +2580,7 @@
         <v>9</v>
       </c>
       <c r="E81" s="1">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>22</v>
@@ -2568,10 +2589,10 @@
         <v>13</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2588,7 +2609,7 @@
         <v>9</v>
       </c>
       <c r="E82" s="1">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>22</v>
@@ -2597,10 +2618,10 @@
         <v>13</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2617,7 +2638,7 @@
         <v>9</v>
       </c>
       <c r="E83" s="1">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>22</v>
@@ -2626,10 +2647,10 @@
         <v>13</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2646,7 +2667,7 @@
         <v>9</v>
       </c>
       <c r="E84" s="1">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>22</v>
@@ -2655,255 +2676,400 @@
         <v>13</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="I85"/>
-      <c r="J85"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="1">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="1">
+        <v>100</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>8</v>
-      </c>
-      <c r="B86">
-        <v>9</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86">
-        <v>25</v>
-      </c>
-      <c r="F86" t="s">
-        <v>22</v>
-      </c>
-      <c r="G86" t="s">
-        <v>13</v>
-      </c>
-      <c r="H86" t="s">
-        <v>29</v>
-      </c>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
       <c r="I86"/>
       <c r="J86"/>
     </row>
-    <row r="87" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="1">
-        <v>9</v>
-      </c>
-      <c r="C87" s="1">
-        <v>1</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="1">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87">
         <v>25</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="F87" t="s">
         <v>22</v>
       </c>
-      <c r="G87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88">
-        <v>9</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88">
+      <c r="G87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H87" t="s">
+        <v>29</v>
+      </c>
+      <c r="I87"/>
+      <c r="J87"/>
+    </row>
+    <row r="88" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="1">
+        <v>9</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>25</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89">
+        <v>9</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89">
         <v>50</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" t="s">
         <v>22</v>
       </c>
-      <c r="G88" t="s">
-        <v>13</v>
-      </c>
-      <c r="H88" t="s">
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" t="s">
         <v>29</v>
       </c>
-      <c r="I88"/>
-      <c r="J88"/>
-    </row>
-    <row r="89" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B89" s="1">
-        <v>9</v>
-      </c>
-      <c r="C89" s="1">
-        <v>1</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="1">
+      <c r="I89"/>
+      <c r="J89"/>
+    </row>
+    <row r="90" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="1">
+        <v>9</v>
+      </c>
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="1">
         <v>50</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J89" s="1" t="s">
+      <c r="G90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90">
-        <v>9</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90">
+      <c r="J90" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91">
         <v>75</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F91" t="s">
         <v>22</v>
       </c>
-      <c r="G90" t="s">
-        <v>13</v>
-      </c>
-      <c r="H90" t="s">
+      <c r="G91" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" t="s">
         <v>29</v>
       </c>
-      <c r="I90"/>
-      <c r="J90"/>
-    </row>
-    <row r="91" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="1">
-        <v>9</v>
-      </c>
-      <c r="C91" s="1">
-        <v>1</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="1">
+      <c r="I91"/>
+      <c r="J91"/>
+    </row>
+    <row r="92" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" s="1">
+        <v>9</v>
+      </c>
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" s="1">
         <v>75</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>8</v>
-      </c>
-      <c r="B92">
-        <v>9</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92">
-        <v>100</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="G92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>100</v>
+      </c>
+      <c r="F93" t="s">
         <v>22</v>
       </c>
-      <c r="G92" t="s">
-        <v>13</v>
-      </c>
-      <c r="H92" t="s">
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" t="s">
         <v>29</v>
       </c>
-      <c r="I92"/>
-      <c r="J92"/>
-    </row>
-    <row r="93" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B93" s="1">
-        <v>9</v>
-      </c>
-      <c r="C93" s="1">
-        <v>1</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="1">
-        <v>100</v>
-      </c>
-      <c r="F93" s="1" t="s">
+      <c r="I93"/>
+      <c r="J93"/>
+    </row>
+    <row r="94" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="1">
+        <v>9</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="1">
+        <v>100</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G93" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>53</v>
+      <c r="G94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="8">
+        <v>8</v>
+      </c>
+      <c r="C97" s="8">
+        <v>2</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="8">
+        <v>25</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="8">
+        <v>8</v>
+      </c>
+      <c r="C98" s="8">
+        <v>2</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" s="8">
+        <v>50</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I98" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="8">
+        <v>8</v>
+      </c>
+      <c r="C99" s="8">
+        <v>2</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" s="8">
+        <v>75</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I99" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="8">
+        <v>8</v>
+      </c>
+      <c r="C100" s="8">
+        <v>2</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" s="8">
+        <v>100</v>
+      </c>
+      <c r="F100" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I100" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINALLY FINISHED TRAFFIC SIGN
</commit_message>
<xml_diff>
--- a/examples/masterarbeit/gtsrb_notebooks/experiments_gtsrb.xlsx
+++ b/examples/masterarbeit/gtsrb_notebooks/experiments_gtsrb.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\PySyft-fork\examples\masterarbeit\gtsrb_notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE291832-0969-453A-A166-42A637870314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF9C21A-7E14-4E75-BFA0-C88AE9825847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11075B9-7AA2-416A-A2BB-E8EDCD451B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="104">
   <si>
     <t>Merge strategy</t>
   </si>
@@ -319,15 +318,9 @@
     <t>exp_gtsrb_20200318-203612</t>
   </si>
   <si>
-    <t>ongoing</t>
-  </si>
-  <si>
     <t>exp_gtsrb_20200319-161053</t>
   </si>
   <si>
-    <t>exp_gtsrb_20200319-173620</t>
-  </si>
-  <si>
     <t>exp_gtsrb_20200320-003449</t>
   </si>
   <si>
@@ -341,6 +334,15 @@
   </si>
   <si>
     <t>exp_gtsrb_20200321-011532</t>
+  </si>
+  <si>
+    <t>REDO</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200321-154836</t>
+  </si>
+  <si>
+    <t>exp_gtsrb_20200321-154705</t>
   </si>
 </sst>
 </file>
@@ -819,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A100B0B-FE3B-4C26-A276-BE253BBFC4CB}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2159,7 +2161,7 @@
         <v>30</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -2188,7 +2190,10 @@
         <v>30</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -2217,7 +2222,7 @@
         <v>30</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -2246,7 +2251,7 @@
         <v>30</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
@@ -2982,7 +2987,7 @@
         <v>30</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -3011,7 +3016,7 @@
         <v>30</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -3040,7 +3045,7 @@
         <v>30</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -3069,7 +3074,7 @@
         <v>30</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>